<commit_message>
update general, machine learning and output images for Task 3
</commit_message>
<xml_diff>
--- a/task_status.xlsx
+++ b/task_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD05EC0-F024-4D2F-9F7E-EBC3AA22C500}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF05E496-7436-4EDB-BC08-95178EEBCF66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>task</t>
   </si>
@@ -241,12 +241,6 @@
     <t xml:space="preserve">GT: nb of ratio_width values unequal to nb of bgr_colors </t>
   </si>
   <si>
-    <t>GT: same ratio_width values not found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">write down how many hours you spent on each of the tasks </t>
-  </si>
-  <si>
     <t>unequal vian color distribution, what to do? alexandra: doesn't matter, linda: as long as the minimum number per class is satisfied</t>
   </si>
   <si>
@@ -274,13 +268,58 @@
     <t xml:space="preserve">overview of tasks: diagram (AD) </t>
   </si>
   <si>
-    <t xml:space="preserve">GT: which ml evaluation score to take? (took accuracy and inverse to get error, but F1 might be better? </t>
-  </si>
-  <si>
     <t xml:space="preserve">machine learning pipeline: knn + svc </t>
   </si>
   <si>
     <t>reorganization of file structure: py script with ordered numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare multidim histograms (opencv, cv2.comparehist() look for similarity metrics ) </t>
+  </si>
+  <si>
+    <t>write down how many hours you spent on each of the tasks / gantt diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT: which ml evaluation score to take? All (took accuracy and inverse to get error, but F1 might be better? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lab histogram </t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do webtool </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extend dic with +-1 interval </t>
+  </si>
+  <si>
+    <t>sort color palettes by ratio_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search for avocado, get avocado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extend dic with google image search, problme with img duplicates? </t>
+  </si>
+  <si>
+    <t>EFFCND Thesaurus-Itten</t>
+  </si>
+  <si>
+    <t>classify color palette to 6 color contrasts</t>
+  </si>
+  <si>
+    <t>color contrast definition</t>
+  </si>
+  <si>
+    <t>search color palettes for a certain color contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOASK: how to define color contrast to revise? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOASK: which contrast schemes? </t>
   </si>
 </sst>
 </file>
@@ -342,7 +381,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +412,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -387,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -400,6 +451,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -681,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1162,153 +1220,275 @@
       <c r="A39">
         <v>42</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="9" t="s">
         <v>55</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>43</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>44</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>45</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E45" t="s">
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>54</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
+        <v>55</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>55</v>
-      </c>
-      <c r="B52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>56</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" t="s">
-        <v>17</v>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>57</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B63" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>